<commit_message>
images on the end of month
</commit_message>
<xml_diff>
--- a/crawler/headpagepb.xlsx
+++ b/crawler/headpagepb.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA179"/>
+  <dimension ref="A1:AA201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -15508,88 +15508,1958 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr">
+      <c r="A179" s="2" t="inlineStr">
         <is>
           <t>2025/8/28</t>
         </is>
       </c>
-      <c r="B179" t="n">
+      <c r="B179" s="2" t="n">
         <v>2.56</v>
       </c>
-      <c r="C179" t="n">
+      <c r="C179" s="2" t="n">
         <v>4.97</v>
       </c>
-      <c r="D179" t="n">
+      <c r="D179" s="2" t="n">
         <v>2.68</v>
       </c>
-      <c r="E179" t="n">
+      <c r="E179" s="2" t="n">
         <v>3.53</v>
       </c>
-      <c r="F179" t="n">
+      <c r="F179" s="2" t="n">
         <v>5.66</v>
       </c>
-      <c r="G179" t="n">
+      <c r="G179" s="2" t="n">
         <v>2.08</v>
       </c>
-      <c r="H179" t="n">
+      <c r="H179" s="2" t="n">
         <v>4.23</v>
       </c>
-      <c r="I179" t="n">
+      <c r="I179" s="2" t="n">
         <v>3.97</v>
       </c>
-      <c r="J179" t="n">
+      <c r="J179" s="2" t="n">
         <v>3.88</v>
       </c>
-      <c r="K179" t="n">
+      <c r="K179" s="2" t="n">
         <v>3.55</v>
       </c>
-      <c r="L179" t="n">
+      <c r="L179" s="2" t="n">
         <v>5.98</v>
       </c>
-      <c r="M179" t="n">
+      <c r="M179" s="2" t="n">
         <v>2.76</v>
       </c>
-      <c r="N179" t="n">
+      <c r="N179" s="2" t="n">
         <v>2.4</v>
       </c>
-      <c r="O179" t="n">
+      <c r="O179" s="2" t="n">
         <v>5.5</v>
       </c>
-      <c r="P179" t="n">
+      <c r="P179" s="2" t="n">
         <v>4.08</v>
       </c>
-      <c r="Q179" t="n">
+      <c r="Q179" s="2" t="n">
         <v>1.58</v>
       </c>
-      <c r="R179" t="n">
+      <c r="R179" s="2" t="n">
         <v>2.65</v>
       </c>
-      <c r="S179" t="n">
+      <c r="S179" s="2" t="n">
         <v>1.8</v>
       </c>
-      <c r="T179" t="n">
+      <c r="T179" s="2" t="n">
         <v>7.36</v>
       </c>
-      <c r="U179" t="n">
+      <c r="U179" s="2" t="n">
         <v>3.64</v>
       </c>
-      <c r="V179" t="n">
+      <c r="V179" s="2" t="n">
         <v>3.28</v>
       </c>
-      <c r="W179" t="n">
+      <c r="W179" s="2" t="n">
         <v>1.52</v>
       </c>
-      <c r="X179" t="n">
+      <c r="X179" s="2" t="n">
         <v>2.03</v>
       </c>
-      <c r="Y179" t="n">
+      <c r="Y179" s="2" t="n">
         <v>6.06</v>
       </c>
-      <c r="Z179" t="n">
+      <c r="Z179" s="2" t="n">
         <v>0.8</v>
       </c>
-      <c r="AA179" t="n">
+      <c r="AA179" s="2" t="n">
         <v>0.91</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="inlineStr">
+        <is>
+          <t>2025/8/29</t>
+        </is>
+      </c>
+      <c r="B180" s="2" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="C180" s="2" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="D180" s="2" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="E180" s="2" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="F180" s="2" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="G180" s="2" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="H180" s="2" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="I180" s="2" t="n">
+        <v>3.96</v>
+      </c>
+      <c r="J180" s="2" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="K180" s="2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="L180" s="2" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="M180" s="2" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="N180" s="2" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="O180" s="2" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="P180" s="2" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="Q180" s="2" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="R180" s="2" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="S180" s="2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="T180" s="2" t="n">
+        <v>7.07</v>
+      </c>
+      <c r="U180" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="V180" s="2" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="W180" s="2" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="X180" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="Y180" s="2" t="n">
+        <v>6.07</v>
+      </c>
+      <c r="Z180" s="2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AA180" s="2" t="n">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/01</t>
+        </is>
+      </c>
+      <c r="B181" s="2" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="C181" s="2" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="D181" s="2" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="E181" s="2" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="F181" s="2" t="n">
+        <v>5.96</v>
+      </c>
+      <c r="G181" s="2" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="H181" s="2" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="I181" s="2" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="J181" s="2" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="K181" s="2" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="L181" s="2" t="n">
+        <v>6.16</v>
+      </c>
+      <c r="M181" s="2" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="N181" s="2" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="O181" s="2" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="P181" s="2" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="Q181" s="2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="R181" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="S181" s="2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="T181" s="2" t="n">
+        <v>7.16</v>
+      </c>
+      <c r="U181" s="2" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="V181" s="2" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="W181" s="2" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="X181" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="Y181" s="2" t="n">
+        <v>6.15</v>
+      </c>
+      <c r="Z181" s="2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="AA181" s="2" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/02</t>
+        </is>
+      </c>
+      <c r="B182" s="2" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="C182" s="2" t="n">
+        <v>5.06</v>
+      </c>
+      <c r="D182" s="2" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="E182" s="2" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="F182" s="2" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="G182" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="H182" s="2" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="I182" s="2" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="J182" s="2" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="K182" s="2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="L182" s="2" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="M182" s="2" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="N182" s="2" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="O182" s="2" t="n">
+        <v>5.64</v>
+      </c>
+      <c r="P182" s="2" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="Q182" s="2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="R182" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="S182" s="2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="T182" s="2" t="n">
+        <v>7.16</v>
+      </c>
+      <c r="U182" s="2" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="V182" s="2" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="W182" s="2" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="X182" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="Y182" s="2" t="n">
+        <v>6.15</v>
+      </c>
+      <c r="Z182" s="2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="AA182" s="2" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/03</t>
+        </is>
+      </c>
+      <c r="B183" s="2" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="C183" s="2" t="n">
+        <v>5.07</v>
+      </c>
+      <c r="D183" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="E183" s="2" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="F183" s="2" t="n">
+        <v>5.84</v>
+      </c>
+      <c r="G183" s="2" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="H183" s="2" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="I183" s="2" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="J183" s="2" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="K183" s="2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="L183" s="2" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="M183" s="2" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="N183" s="2" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="O183" s="2" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="P183" s="2" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="Q183" s="2" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="R183" s="2" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="S183" s="2" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="T183" s="2" t="n">
+        <v>6.83</v>
+      </c>
+      <c r="U183" s="2" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="V183" s="2" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="W183" s="2" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="X183" s="2" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="Y183" s="2" t="n">
+        <v>5.81</v>
+      </c>
+      <c r="Z183" s="2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AA183" s="2" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/04</t>
+        </is>
+      </c>
+      <c r="B184" s="2" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="C184" s="2" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="D184" s="2" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E184" s="2" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="F184" s="2" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="G184" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H184" s="2" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="I184" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="J184" s="2" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="K184" s="2" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="L184" s="2" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="M184" s="2" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="N184" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="O184" s="2" t="n">
+        <v>5.43</v>
+      </c>
+      <c r="P184" s="2" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="Q184" s="2" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="R184" s="2" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="S184" s="2" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="T184" s="2" t="n">
+        <v>6.29</v>
+      </c>
+      <c r="U184" s="2" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="V184" s="2" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="W184" s="2" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="X184" s="2" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="Y184" s="2" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="Z184" s="2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AA184" s="2" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/05</t>
+        </is>
+      </c>
+      <c r="B185" s="2" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="C185" s="2" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="D185" s="2" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="E185" s="2" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="F185" s="2" t="n">
+        <v>5.96</v>
+      </c>
+      <c r="G185" s="2" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="H185" s="2" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="I185" s="2" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="J185" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="K185" s="2" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="L185" s="2" t="n">
+        <v>5.72</v>
+      </c>
+      <c r="M185" s="2" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="N185" s="2" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="O185" s="2" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="P185" s="2" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="Q185" s="2" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="R185" s="2" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="S185" s="2" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="T185" s="2" t="n">
+        <v>6.51</v>
+      </c>
+      <c r="U185" s="2" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="V185" s="2" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="W185" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="X185" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="Y185" s="2" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="Z185" s="2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AA185" s="2" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/08</t>
+        </is>
+      </c>
+      <c r="B186" s="2" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="C186" s="2" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="D186" s="2" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E186" s="2" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="F186" s="2" t="n">
+        <v>5.91</v>
+      </c>
+      <c r="G186" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="H186" s="2" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="I186" s="2" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="J186" s="2" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="K186" s="2" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="L186" s="2" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="M186" s="2" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="N186" s="2" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="O186" s="2" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="P186" s="2" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="Q186" s="2" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="R186" s="2" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="S186" s="2" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="T186" s="2" t="n">
+        <v>6.53</v>
+      </c>
+      <c r="U186" s="2" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="V186" s="2" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="W186" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="X186" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="Y186" s="2" t="n">
+        <v>5.57</v>
+      </c>
+      <c r="Z186" s="2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AA186" s="2" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/09</t>
+        </is>
+      </c>
+      <c r="B187" s="2" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="C187" s="2" t="n">
+        <v>5.03</v>
+      </c>
+      <c r="D187" s="2" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="E187" s="2" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="F187" s="2" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="G187" s="2" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="H187" s="2" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="I187" s="2" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="J187" s="2" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="K187" s="2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="L187" s="2" t="n">
+        <v>5.55</v>
+      </c>
+      <c r="M187" s="2" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="N187" s="2" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="O187" s="2" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="P187" s="2" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="Q187" s="2" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="R187" s="2" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="S187" s="2" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="T187" s="2" t="n">
+        <v>6.36</v>
+      </c>
+      <c r="U187" s="2" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="V187" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="W187" s="2" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="X187" s="2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="Y187" s="2" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="Z187" s="2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AA187" s="2" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/10</t>
+        </is>
+      </c>
+      <c r="B188" s="2" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="C188" s="2" t="n">
+        <v>5.07</v>
+      </c>
+      <c r="D188" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="E188" s="2" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="F188" s="2" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="G188" s="2" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="H188" s="2" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="I188" s="2" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="J188" s="2" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="K188" s="2" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="L188" s="2" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="M188" s="2" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="N188" s="2" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="O188" s="2" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="P188" s="2" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="Q188" s="2" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="R188" s="2" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="S188" s="2" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="T188" s="2" t="n">
+        <v>6.49</v>
+      </c>
+      <c r="U188" s="2" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="V188" s="2" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="W188" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="X188" s="2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="Y188" s="2" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="Z188" s="2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AA188" s="2" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/11</t>
+        </is>
+      </c>
+      <c r="B189" s="2" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="C189" s="2" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="D189" s="2" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="E189" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="F189" s="2" t="n">
+        <v>6.13</v>
+      </c>
+      <c r="G189" s="2" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="H189" s="2" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="I189" s="2" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="J189" s="2" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="K189" s="2" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="L189" s="2" t="n">
+        <v>6.03</v>
+      </c>
+      <c r="M189" s="2" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="N189" s="2" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="O189" s="2" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="P189" s="2" t="n">
+        <v>4.34</v>
+      </c>
+      <c r="Q189" s="2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="R189" s="2" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="S189" s="2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="T189" s="2" t="n">
+        <v>6.95</v>
+      </c>
+      <c r="U189" s="2" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="V189" s="2" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="W189" s="2" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="X189" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="Y189" s="2" t="n">
+        <v>5.96</v>
+      </c>
+      <c r="Z189" s="2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AA189" s="2" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/12</t>
+        </is>
+      </c>
+      <c r="B190" s="2" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="C190" s="2" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="D190" s="2" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="E190" s="2" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="F190" s="2" t="n">
+        <v>6.07</v>
+      </c>
+      <c r="G190" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="H190" s="2" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="I190" s="2" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="J190" s="2" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="K190" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="L190" s="2" t="n">
+        <v>5.97</v>
+      </c>
+      <c r="M190" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="N190" s="2" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="O190" s="2" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="P190" s="2" t="n">
+        <v>4.31</v>
+      </c>
+      <c r="Q190" s="2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="R190" s="2" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="S190" s="2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="T190" s="2" t="n">
+        <v>7.06</v>
+      </c>
+      <c r="U190" s="2" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="V190" s="2" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="W190" s="2" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="X190" s="2" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="Y190" s="2" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="Z190" s="2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AA190" s="2" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/15</t>
+        </is>
+      </c>
+      <c r="B191" s="2" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="C191" s="2" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="D191" s="2" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="E191" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="F191" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="G191" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="H191" s="2" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="I191" s="2" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="J191" s="2" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="K191" s="2" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="L191" s="2" t="n">
+        <v>5.97</v>
+      </c>
+      <c r="M191" s="2" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="N191" s="2" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="O191" s="2" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="P191" s="2" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="Q191" s="2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="R191" s="2" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="S191" s="2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="T191" s="2" t="n">
+        <v>7.12</v>
+      </c>
+      <c r="U191" s="2" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="V191" s="2" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="W191" s="2" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="X191" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="Y191" s="2" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="Z191" s="2" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="AA191" s="2" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/16</t>
+        </is>
+      </c>
+      <c r="B192" s="2" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="C192" s="2" t="n">
+        <v>5.37</v>
+      </c>
+      <c r="D192" s="2" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="E192" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="F192" s="2" t="n">
+        <v>6.23</v>
+      </c>
+      <c r="G192" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="H192" s="2" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="I192" s="2" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="J192" s="2" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="K192" s="2" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="L192" s="2" t="n">
+        <v>6.03</v>
+      </c>
+      <c r="M192" s="2" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="N192" s="2" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="O192" s="2" t="n">
+        <v>6.43</v>
+      </c>
+      <c r="P192" s="2" t="n">
+        <v>4.39</v>
+      </c>
+      <c r="Q192" s="2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="R192" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="S192" s="2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="T192" s="2" t="n">
+        <v>7.23</v>
+      </c>
+      <c r="U192" s="2" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="V192" s="2" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="W192" s="2" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="X192" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="Y192" s="2" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="Z192" s="2" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="AA192" s="2" t="n">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/17</t>
+        </is>
+      </c>
+      <c r="B193" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="C193" s="2" t="n">
+        <v>5.47</v>
+      </c>
+      <c r="D193" s="2" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="E193" s="2" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="F193" s="2" t="n">
+        <v>6.37</v>
+      </c>
+      <c r="G193" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="H193" s="2" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="I193" s="2" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="J193" s="2" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="K193" s="2" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="L193" s="2" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="M193" s="2" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="N193" s="2" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="O193" s="2" t="n">
+        <v>6.57</v>
+      </c>
+      <c r="P193" s="2" t="n">
+        <v>4.47</v>
+      </c>
+      <c r="Q193" s="2" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="R193" s="2" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="S193" s="2" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="T193" s="2" t="n">
+        <v>7.29</v>
+      </c>
+      <c r="U193" s="2" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="V193" s="2" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="W193" s="2" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="X193" s="2" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="Y193" s="2" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="Z193" s="2" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="AA193" s="2" t="n">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/18</t>
+        </is>
+      </c>
+      <c r="B194" s="2" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="C194" s="2" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="D194" s="2" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="E194" s="2" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="F194" s="2" t="n">
+        <v>6.26</v>
+      </c>
+      <c r="G194" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="H194" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I194" s="2" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="J194" s="2" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="K194" s="2" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="L194" s="2" t="n">
+        <v>6.07</v>
+      </c>
+      <c r="M194" s="2" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="N194" s="2" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="O194" s="2" t="n">
+        <v>6.47</v>
+      </c>
+      <c r="P194" s="2" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="Q194" s="2" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="R194" s="2" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="S194" s="2" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="T194" s="2" t="n">
+        <v>7.42</v>
+      </c>
+      <c r="U194" s="2" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="V194" s="2" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="W194" s="2" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="X194" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="Y194" s="2" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="Z194" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="AA194" s="2" t="n">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/19</t>
+        </is>
+      </c>
+      <c r="B195" s="2" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="C195" s="2" t="n">
+        <v>5.38</v>
+      </c>
+      <c r="D195" s="2" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="E195" s="2" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="F195" s="2" t="n">
+        <v>6.26</v>
+      </c>
+      <c r="G195" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="H195" s="2" t="n">
+        <v>4.58</v>
+      </c>
+      <c r="I195" s="2" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="J195" s="2" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="K195" s="2" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="L195" s="2" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="M195" s="2" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="N195" s="2" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="O195" s="2" t="n">
+        <v>6.46</v>
+      </c>
+      <c r="P195" s="2" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="Q195" s="2" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="R195" s="2" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="S195" s="2" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="T195" s="2" t="n">
+        <v>7.27</v>
+      </c>
+      <c r="U195" s="2" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="V195" s="2" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="W195" s="2" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="X195" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="Y195" s="2" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="Z195" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="AA195" s="2" t="n">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/22</t>
+        </is>
+      </c>
+      <c r="B196" s="2" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="C196" s="2" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="D196" s="2" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="E196" s="2" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="F196" s="2" t="n">
+        <v>6.31</v>
+      </c>
+      <c r="G196" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="H196" s="2" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="I196" s="2" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="J196" s="2" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="K196" s="2" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="L196" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="M196" s="2" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="N196" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="O196" s="2" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="P196" s="2" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="Q196" s="2" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="R196" s="2" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="S196" s="2" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="T196" s="2" t="n">
+        <v>7.59</v>
+      </c>
+      <c r="U196" s="2" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="V196" s="2" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="W196" s="2" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="X196" s="2" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="Y196" s="2" t="n">
+        <v>6.04</v>
+      </c>
+      <c r="Z196" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AA196" s="2" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/23</t>
+        </is>
+      </c>
+      <c r="B197" s="2" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="C197" s="2" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="D197" s="2" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="E197" s="2" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="F197" s="2" t="n">
+        <v>6.33</v>
+      </c>
+      <c r="G197" s="2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="H197" s="2" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="I197" s="2" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="J197" s="2" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="K197" s="2" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="L197" s="2" t="n">
+        <v>6.15</v>
+      </c>
+      <c r="M197" s="2" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="N197" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="O197" s="2" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="P197" s="2" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="Q197" s="2" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="R197" s="2" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="S197" s="2" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="T197" s="2" t="n">
+        <v>7.57</v>
+      </c>
+      <c r="U197" s="2" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="V197" s="2" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="W197" s="2" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="X197" s="2" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="Y197" s="2" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="Z197" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="AA197" s="2" t="n">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/24</t>
+        </is>
+      </c>
+      <c r="B198" s="2" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="C198" s="2" t="n">
+        <v>5.53</v>
+      </c>
+      <c r="D198" s="2" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="E198" s="2" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="F198" s="2" t="n">
+        <v>6.47</v>
+      </c>
+      <c r="G198" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H198" s="2" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="I198" s="2" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="J198" s="2" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="K198" s="2" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="L198" s="2" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="M198" s="2" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="N198" s="2" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="O198" s="2" t="n">
+        <v>6.64</v>
+      </c>
+      <c r="P198" s="2" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="Q198" s="2" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="R198" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="S198" s="2" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="T198" s="2" t="n">
+        <v>7.89</v>
+      </c>
+      <c r="U198" s="2" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="V198" s="2" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="W198" s="2" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="X198" s="2" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="Y198" s="2" t="n">
+        <v>6.07</v>
+      </c>
+      <c r="Z198" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="AA198" s="2" t="n">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/25</t>
+        </is>
+      </c>
+      <c r="B199" s="2" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="C199" s="2" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="D199" s="2" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="E199" s="2" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="F199" s="2" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="G199" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H199" s="2" t="n">
+        <v>4.81</v>
+      </c>
+      <c r="I199" s="2" t="n">
+        <v>3.96</v>
+      </c>
+      <c r="J199" s="2" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="K199" s="2" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="L199" s="2" t="n">
+        <v>6.35</v>
+      </c>
+      <c r="M199" s="2" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="N199" s="2" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="O199" s="2" t="n">
+        <v>6.77</v>
+      </c>
+      <c r="P199" s="2" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="Q199" s="2" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="R199" s="2" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="S199" s="2" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="T199" s="2" t="n">
+        <v>7.96</v>
+      </c>
+      <c r="U199" s="2" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="V199" s="2" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="W199" s="2" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="X199" s="2" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="Y199" s="2" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="Z199" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="AA199" s="2" t="n">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="2" t="inlineStr">
+        <is>
+          <t>2025/9/26</t>
+        </is>
+      </c>
+      <c r="B200" s="2" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="C200" s="2" t="n">
+        <v>5.48</v>
+      </c>
+      <c r="D200" s="2" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="E200" s="2" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="F200" s="2" t="n">
+        <v>6.42</v>
+      </c>
+      <c r="G200" s="2" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="H200" s="2" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="I200" s="2" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="J200" s="2" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="K200" s="2" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="L200" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="M200" s="2" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="N200" s="2" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="O200" s="2" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="P200" s="2" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="Q200" s="2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="R200" s="2" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="S200" s="2" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="T200" s="2" t="n">
+        <v>7.85</v>
+      </c>
+      <c r="U200" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="V200" s="2" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="W200" s="2" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="X200" s="2" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="Y200" s="2" t="n">
+        <v>5.96</v>
+      </c>
+      <c r="Z200" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="AA200" s="2" t="n">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2025/9/29</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="C201" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="D201" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="E201" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="F201" t="n">
+        <v>6.61</v>
+      </c>
+      <c r="G201" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H201" t="n">
+        <v>4.81</v>
+      </c>
+      <c r="I201" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="J201" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="K201" t="n">
+        <v>4.06</v>
+      </c>
+      <c r="L201" t="n">
+        <v>6.32</v>
+      </c>
+      <c r="M201" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="N201" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="O201" t="n">
+        <v>6.77</v>
+      </c>
+      <c r="P201" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="Q201" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="R201" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="S201" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="T201" t="n">
+        <v>7.93</v>
+      </c>
+      <c r="U201" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="V201" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="W201" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="X201" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="Y201" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="Z201" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="AA201" t="n">
+        <v>0.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>